<commit_message>
fix location issue && add amplifier count
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEE135F-60FA-41EC-B64D-77D54CA59099}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DAD367-F3A6-426E-91AD-FECDE00C6C5C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="76">
   <si>
     <t>发布日期</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -291,6 +291,10 @@
   </si>
   <si>
     <t>视频信息</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>谢天笑</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -849,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
@@ -1097,74 +1101,49 @@
         <v>0</v>
       </c>
       <c r="I3" s="23">
-        <v>2.7777777777777779E-3</v>
+        <v>1.5740740740740741E-3</v>
       </c>
       <c r="J3" s="25">
         <f>(MINUTE(I3)*60+SECOND(I3))-(MINUTE(H3)*60+SECOND(H3))</f>
-        <v>240</v>
+        <v>136</v>
       </c>
       <c r="K3" s="21">
         <v>1</v>
       </c>
       <c r="L3" s="24">
         <f>J3*K3*15/60</f>
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="M3" s="21"/>
-      <c r="N3" s="23">
-        <v>0</v>
-      </c>
-      <c r="O3" s="23">
-        <v>2.7777777777777779E-3</v>
-      </c>
-      <c r="P3" s="25">
-        <f>(MINUTE(O3)*60+SECOND(O3))-(MINUTE(N3)*60+SECOND(N3))</f>
-        <v>240</v>
-      </c>
-      <c r="Q3" s="21">
-        <v>1</v>
-      </c>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="21"/>
       <c r="R3" s="24">
         <f>P3*Q3*15/60</f>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="S3" s="21"/>
-      <c r="T3" s="23">
-        <v>2.7777777777777779E-3</v>
-      </c>
-      <c r="U3" s="23">
-        <v>5.5555555555555558E-3</v>
-      </c>
-      <c r="V3" s="25">
-        <f>(MINUTE(U3)*60+SECOND(U3))-(MINUTE(T3)*60+SECOND(T3))</f>
-        <v>240</v>
-      </c>
-      <c r="W3" s="21">
-        <v>1</v>
-      </c>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="21"/>
       <c r="X3" s="24">
         <f>V3*W3*15/60</f>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="21"/>
-      <c r="Z3" s="23">
-        <v>5.5555555555555558E-3</v>
-      </c>
-      <c r="AA3" s="23">
-        <v>1.0023148148148147E-2</v>
-      </c>
-      <c r="AB3" s="25">
-        <f>(MINUTE(AA3)*60+SECOND(AA3))-(MINUTE(Z3)*60+SECOND(Z3))</f>
-        <v>386</v>
-      </c>
-      <c r="AC3" s="21">
-        <v>1</v>
-      </c>
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="25"/>
+      <c r="AC3" s="21"/>
       <c r="AD3" s="24">
         <f>AB3*AC3*15/60</f>
-        <v>96.5</v>
-      </c>
-      <c r="AE3" s="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE3" s="21" t="s">
+        <v>75</v>
+      </c>
       <c r="AF3" s="21">
         <f>IF(K3=0.8,L3*0.2,0)+IF(Q3=0.8,R3*0.2,0)+IF(W3=0.8,X3*0.2,0)+IF(AC3=0.8,AD3*0.2,0)</f>
         <v>0</v>
@@ -1189,7 +1168,7 @@
       </c>
       <c r="AL3" s="24">
         <f t="shared" ref="AL3:AL10" si="0">AI3+AK3+AG3+AD3+X3+R3+L3+F3</f>
-        <v>360.9666666666667</v>
+        <v>118.46666666666667</v>
       </c>
       <c r="AM3" s="27"/>
       <c r="AN3" s="27"/>
@@ -1259,13 +1238,19 @@
       <c r="U4" s="23"/>
       <c r="V4" s="25"/>
       <c r="W4" s="21"/>
-      <c r="X4" s="24"/>
+      <c r="X4" s="24">
+        <f t="shared" ref="X4:X9" si="1">V4*W4*15/60</f>
+        <v>0</v>
+      </c>
       <c r="Y4" s="21"/>
       <c r="Z4" s="23"/>
       <c r="AA4" s="23"/>
       <c r="AB4" s="25"/>
       <c r="AC4" s="21"/>
-      <c r="AD4" s="24"/>
+      <c r="AD4" s="24">
+        <f t="shared" ref="AD4:AD10" si="2">AB4*AC4*15/60</f>
+        <v>0</v>
+      </c>
       <c r="AE4" s="21" t="s">
         <v>30</v>
       </c>
@@ -1315,7 +1300,7 @@
         <v>29</v>
       </c>
       <c r="F5" s="24">
-        <f t="shared" ref="F5:F10" si="1">(MINUTE(D5)*60+SECOND(D5))*3/60</f>
+        <f t="shared" ref="F5:F10" si="3">(MINUTE(D5)*60+SECOND(D5))*3/60</f>
         <v>34.049999999999997</v>
       </c>
       <c r="G5" s="21" t="s">
@@ -1328,14 +1313,14 @@
         <v>7.8819444444444432E-3</v>
       </c>
       <c r="J5" s="25">
-        <f t="shared" ref="J5:J10" si="2">(MINUTE(I5)*60+SECOND(I5))-(MINUTE(H5)*60+SECOND(H5))</f>
+        <f t="shared" ref="J5:J10" si="4">(MINUTE(I5)*60+SECOND(I5))-(MINUTE(H5)*60+SECOND(H5))</f>
         <v>681</v>
       </c>
       <c r="K5" s="21">
         <v>0.8</v>
       </c>
       <c r="L5" s="24">
-        <f t="shared" ref="L5:L10" si="3">J5*K5*15/60</f>
+        <f t="shared" ref="L5:L10" si="5">J5*K5*15/60</f>
         <v>136.20000000000002</v>
       </c>
       <c r="M5" s="21"/>
@@ -1343,28 +1328,37 @@
       <c r="O5" s="23"/>
       <c r="P5" s="25"/>
       <c r="Q5" s="21"/>
-      <c r="R5" s="24"/>
+      <c r="R5" s="24">
+        <f t="shared" ref="R5:R10" si="6">P5*Q5*15/60</f>
+        <v>0</v>
+      </c>
       <c r="S5" s="21"/>
       <c r="T5" s="23"/>
       <c r="U5" s="23"/>
       <c r="V5" s="25"/>
       <c r="W5" s="21"/>
-      <c r="X5" s="24"/>
+      <c r="X5" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Y5" s="21"/>
       <c r="Z5" s="23"/>
       <c r="AA5" s="23"/>
       <c r="AB5" s="25"/>
       <c r="AC5" s="21"/>
-      <c r="AD5" s="24"/>
+      <c r="AD5" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="AE5" s="21" t="s">
         <v>29</v>
       </c>
       <c r="AF5" s="21">
-        <f t="shared" ref="AF5:AF10" si="4">IF(K5=0.8,L5*0.2,0)+IF(Q5=0.8,R5*0.2,0)+IF(W5=0.8,X5*0.2,0)+IF(AC5=0.8,AD5*0.2,0)</f>
+        <f t="shared" ref="AF5:AF10" si="7">IF(K5=0.8,L5*0.2,0)+IF(Q5=0.8,R5*0.2,0)+IF(W5=0.8,X5*0.2,0)+IF(AC5=0.8,AD5*0.2,0)</f>
         <v>27.240000000000006</v>
       </c>
       <c r="AG5" s="24">
-        <f t="shared" ref="AG5:AG10" si="5">(MINUTE(D5)*60+SECOND(D5))*10/60</f>
+        <f t="shared" ref="AG5:AG10" si="8">(MINUTE(D5)*60+SECOND(D5))*10/60</f>
         <v>113.5</v>
       </c>
       <c r="AH5" s="21" t="s">
@@ -1405,7 +1399,7 @@
         <v>30</v>
       </c>
       <c r="F6" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>41.55</v>
       </c>
       <c r="G6" s="21" t="s">
@@ -1418,14 +1412,14 @@
         <v>2.4189814814814816E-3</v>
       </c>
       <c r="J6" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>209</v>
       </c>
       <c r="K6" s="21">
         <v>0.8</v>
       </c>
       <c r="L6" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41.800000000000004</v>
       </c>
       <c r="M6" s="21" t="s">
@@ -1438,14 +1432,14 @@
         <v>4.8495370370370368E-3</v>
       </c>
       <c r="P6" s="25">
-        <f t="shared" ref="P6:P10" si="6">(MINUTE(O6)*60+SECOND(O6))-(MINUTE(N6)*60+SECOND(N6))</f>
+        <f t="shared" ref="P6:P10" si="9">(MINUTE(O6)*60+SECOND(O6))-(MINUTE(N6)*60+SECOND(N6))</f>
         <v>209</v>
       </c>
       <c r="Q6" s="21">
         <v>1</v>
       </c>
       <c r="R6" s="24">
-        <f t="shared" ref="R6:R10" si="7">P6*Q6*15/60</f>
+        <f t="shared" si="6"/>
         <v>52.25</v>
       </c>
       <c r="S6" s="21" t="s">
@@ -1458,14 +1452,14 @@
         <v>7.2800925925925915E-3</v>
       </c>
       <c r="V6" s="25">
-        <f t="shared" ref="V6:V10" si="8">(MINUTE(U6)*60+SECOND(U6))-(MINUTE(T6)*60+SECOND(T6))</f>
+        <f t="shared" ref="V6:V10" si="10">(MINUTE(U6)*60+SECOND(U6))-(MINUTE(T6)*60+SECOND(T6))</f>
         <v>209</v>
       </c>
       <c r="W6" s="21">
         <v>1</v>
       </c>
       <c r="X6" s="24">
-        <f t="shared" ref="X6:X10" si="9">V6*W6*15/60</f>
+        <f t="shared" si="1"/>
         <v>52.25</v>
       </c>
       <c r="Y6" s="21" t="s">
@@ -1478,25 +1472,25 @@
         <v>9.4444444444444445E-3</v>
       </c>
       <c r="AB6" s="25">
-        <f t="shared" ref="AB6:AB8" si="10">(MINUTE(AA6)*60+SECOND(AA6))-(MINUTE(Z6)*60+SECOND(Z6))</f>
+        <f t="shared" ref="AB6:AB8" si="11">(MINUTE(AA6)*60+SECOND(AA6))-(MINUTE(Z6)*60+SECOND(Z6))</f>
         <v>186</v>
       </c>
       <c r="AC6" s="21">
         <v>1</v>
       </c>
       <c r="AD6" s="24">
-        <f t="shared" ref="AD6:AD10" si="11">AB6*AC6*15/60</f>
+        <f t="shared" si="2"/>
         <v>46.5</v>
       </c>
       <c r="AE6" s="21" t="s">
         <v>30</v>
       </c>
       <c r="AF6" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.3600000000000012</v>
       </c>
       <c r="AG6" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>138.5</v>
       </c>
       <c r="AH6" s="21" t="s">
@@ -1537,7 +1531,7 @@
         <v>29</v>
       </c>
       <c r="F7" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>14.05</v>
       </c>
       <c r="G7" s="21" t="s">
@@ -1550,14 +1544,14 @@
         <v>3.2523148148148151E-3</v>
       </c>
       <c r="J7" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>281</v>
       </c>
       <c r="K7" s="21">
         <v>1</v>
       </c>
       <c r="L7" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>70.25</v>
       </c>
       <c r="M7" s="21"/>
@@ -1565,28 +1559,37 @@
       <c r="O7" s="23"/>
       <c r="P7" s="25"/>
       <c r="Q7" s="21"/>
-      <c r="R7" s="24"/>
+      <c r="R7" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="S7" s="21"/>
       <c r="T7" s="23"/>
       <c r="U7" s="23"/>
       <c r="V7" s="25"/>
       <c r="W7" s="21"/>
-      <c r="X7" s="24"/>
+      <c r="X7" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Y7" s="21"/>
       <c r="Z7" s="23"/>
       <c r="AA7" s="23"/>
       <c r="AB7" s="25"/>
       <c r="AC7" s="21"/>
-      <c r="AD7" s="24"/>
+      <c r="AD7" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="AE7" s="21" t="s">
         <v>31</v>
       </c>
       <c r="AF7" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AG7" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>46.833333333333336</v>
       </c>
       <c r="AH7" s="21" t="s">
@@ -1627,7 +1630,7 @@
         <v>30</v>
       </c>
       <c r="F8" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>39.950000000000003</v>
       </c>
       <c r="G8" s="21" t="s">
@@ -1640,14 +1643,14 @@
         <v>2.2569444444444447E-3</v>
       </c>
       <c r="J8" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>195</v>
       </c>
       <c r="K8" s="21">
         <v>1</v>
       </c>
       <c r="L8" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>48.75</v>
       </c>
       <c r="M8" s="21" t="s">
@@ -1660,14 +1663,14 @@
         <v>4.5138888888888893E-3</v>
       </c>
       <c r="P8" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>194</v>
       </c>
       <c r="Q8" s="21">
         <v>0.8</v>
       </c>
       <c r="R8" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>38.800000000000004</v>
       </c>
       <c r="S8" s="21" t="s">
@@ -1687,7 +1690,7 @@
         <v>1</v>
       </c>
       <c r="X8" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>48.5</v>
       </c>
       <c r="Y8" s="21" t="s">
@@ -1700,25 +1703,25 @@
         <v>9.0972222222222218E-3</v>
       </c>
       <c r="AB8" s="25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>200</v>
       </c>
       <c r="AC8" s="21">
         <v>0.8</v>
       </c>
       <c r="AD8" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="AE8" s="21" t="s">
         <v>29</v>
       </c>
       <c r="AF8" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>15.760000000000002</v>
       </c>
       <c r="AG8" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>133.16666666666666</v>
       </c>
       <c r="AH8" s="21" t="s">
@@ -1759,7 +1762,7 @@
         <v>38</v>
       </c>
       <c r="F9" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>34.65</v>
       </c>
       <c r="G9" s="21" t="s">
@@ -1772,14 +1775,14 @@
         <v>2.5462962962962961E-3</v>
       </c>
       <c r="J9" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>220</v>
       </c>
       <c r="K9" s="21">
         <v>1</v>
       </c>
       <c r="L9" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>55</v>
       </c>
       <c r="M9" s="21" t="s">
@@ -1792,14 +1795,14 @@
         <v>5.0925925925925921E-3</v>
       </c>
       <c r="P9" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>220</v>
       </c>
       <c r="Q9" s="21">
         <v>1</v>
       </c>
       <c r="R9" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="S9" s="21" t="s">
@@ -1812,14 +1815,14 @@
         <v>7.858796296296296E-3</v>
       </c>
       <c r="V9" s="25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>239</v>
       </c>
       <c r="W9" s="21">
         <v>1</v>
       </c>
       <c r="X9" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>59.75</v>
       </c>
       <c r="Y9" s="21"/>
@@ -1828,18 +1831,18 @@
       <c r="AB9" s="25"/>
       <c r="AC9" s="21"/>
       <c r="AD9" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE9" s="21" t="s">
         <v>31</v>
       </c>
       <c r="AF9" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AG9" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>115.5</v>
       </c>
       <c r="AH9" s="21" t="s">
@@ -1880,7 +1883,7 @@
         <v>29</v>
       </c>
       <c r="F10" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>37.6</v>
       </c>
       <c r="G10" s="21" t="s">
@@ -1893,14 +1896,14 @@
         <v>2.7777777777777801E-3</v>
       </c>
       <c r="J10" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>240</v>
       </c>
       <c r="K10" s="21">
         <v>1</v>
       </c>
       <c r="L10" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="M10" s="21" t="s">
@@ -1913,14 +1916,14 @@
         <v>5.5555555555555558E-3</v>
       </c>
       <c r="P10" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>240</v>
       </c>
       <c r="Q10" s="21">
         <v>0.8</v>
       </c>
       <c r="R10" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
       <c r="S10" s="21" t="s">
@@ -1933,14 +1936,14 @@
         <v>8.5416666666666679E-3</v>
       </c>
       <c r="V10" s="25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>258</v>
       </c>
       <c r="W10" s="21">
         <v>1</v>
       </c>
       <c r="X10" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="X6:X10" si="12">V10*W10*15/60</f>
         <v>64.5</v>
       </c>
       <c r="Y10" s="21"/>
@@ -1949,18 +1952,18 @@
       <c r="AB10" s="25"/>
       <c r="AC10" s="21"/>
       <c r="AD10" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE10" s="21" t="s">
         <v>29</v>
       </c>
       <c r="AF10" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9.6000000000000014</v>
       </c>
       <c r="AG10" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>125.33333333333333</v>
       </c>
       <c r="AH10" s="21" t="s">

</xml_diff>

<commit_message>
fix errors && add features && removed outdated
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DAD367-F3A6-426E-91AD-FECDE00C6C5C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AEE0CE-4E1F-431F-B3F0-C75681932DA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -853,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
@@ -1115,7 +1115,10 @@
         <v>34</v>
       </c>
       <c r="M3" s="21"/>
-      <c r="N3" s="23"/>
+      <c r="N3" s="23">
+        <f>I3</f>
+        <v>1.5740740740740741E-3</v>
+      </c>
       <c r="O3" s="23"/>
       <c r="P3" s="25"/>
       <c r="Q3" s="21"/>
@@ -1124,7 +1127,10 @@
         <v>0</v>
       </c>
       <c r="S3" s="21"/>
-      <c r="T3" s="23"/>
+      <c r="T3" s="23">
+        <f>O3</f>
+        <v>0</v>
+      </c>
       <c r="U3" s="23"/>
       <c r="V3" s="25"/>
       <c r="W3" s="21"/>
@@ -1133,7 +1139,10 @@
         <v>0</v>
       </c>
       <c r="Y3" s="21"/>
-      <c r="Z3" s="23"/>
+      <c r="Z3" s="23">
+        <f>U3</f>
+        <v>0</v>
+      </c>
       <c r="AA3" s="23"/>
       <c r="AB3" s="25"/>
       <c r="AC3" s="21"/>
@@ -1149,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="AG3" s="24">
-        <f>(MINUTE(D3)*60+SECOND(D3))*10/60</f>
+        <f>(MINUTE(D3)*60+SECOND(D3))*10/60+AF3</f>
         <v>22.666666666666668</v>
       </c>
       <c r="AH3" s="21" t="s">
@@ -1217,6 +1226,7 @@
         <v>31</v>
       </c>
       <c r="N4" s="23">
+        <f t="shared" ref="N4:N10" si="1">I4</f>
         <v>2.0833333333333333E-3</v>
       </c>
       <c r="O4" s="23">
@@ -1234,21 +1244,27 @@
         <v>49.75</v>
       </c>
       <c r="S4" s="21"/>
-      <c r="T4" s="23"/>
+      <c r="T4" s="23">
+        <f t="shared" ref="T4:T10" si="2">O4</f>
+        <v>4.386574074074074E-3</v>
+      </c>
       <c r="U4" s="23"/>
       <c r="V4" s="25"/>
       <c r="W4" s="21"/>
       <c r="X4" s="24">
-        <f t="shared" ref="X4:X9" si="1">V4*W4*15/60</f>
+        <f t="shared" ref="X4:X9" si="3">V4*W4*15/60</f>
         <v>0</v>
       </c>
       <c r="Y4" s="21"/>
-      <c r="Z4" s="23"/>
+      <c r="Z4" s="23">
+        <f t="shared" ref="Z4:Z10" si="4">U4</f>
+        <v>0</v>
+      </c>
       <c r="AA4" s="23"/>
       <c r="AB4" s="25"/>
       <c r="AC4" s="21"/>
       <c r="AD4" s="24">
-        <f t="shared" ref="AD4:AD10" si="2">AB4*AC4*15/60</f>
+        <f t="shared" ref="AD4:AD10" si="5">AB4*AC4*15/60</f>
         <v>0</v>
       </c>
       <c r="AE4" s="21" t="s">
@@ -1259,8 +1275,8 @@
         <v>7.2</v>
       </c>
       <c r="AG4" s="24">
-        <f>(MINUTE(D4)*60+SECOND(D4))*10/60</f>
-        <v>63.166666666666664</v>
+        <f t="shared" ref="AG4:AG10" si="6">(MINUTE(D4)*60+SECOND(D4))*10/60+AF4</f>
+        <v>70.36666666666666</v>
       </c>
       <c r="AH4" s="21" t="s">
         <v>32</v>
@@ -1278,7 +1294,7 @@
       </c>
       <c r="AL4" s="24">
         <f t="shared" si="0"/>
-        <v>222.86666666666665</v>
+        <v>230.06666666666666</v>
       </c>
       <c r="AM4" s="27"/>
       <c r="AN4" s="27"/>
@@ -1300,7 +1316,7 @@
         <v>29</v>
       </c>
       <c r="F5" s="24">
-        <f t="shared" ref="F5:F10" si="3">(MINUTE(D5)*60+SECOND(D5))*3/60</f>
+        <f t="shared" ref="F5:F10" si="7">(MINUTE(D5)*60+SECOND(D5))*3/60</f>
         <v>34.049999999999997</v>
       </c>
       <c r="G5" s="21" t="s">
@@ -1313,53 +1329,62 @@
         <v>7.8819444444444432E-3</v>
       </c>
       <c r="J5" s="25">
-        <f t="shared" ref="J5:J10" si="4">(MINUTE(I5)*60+SECOND(I5))-(MINUTE(H5)*60+SECOND(H5))</f>
+        <f t="shared" ref="J5:J10" si="8">(MINUTE(I5)*60+SECOND(I5))-(MINUTE(H5)*60+SECOND(H5))</f>
         <v>681</v>
       </c>
       <c r="K5" s="21">
         <v>0.8</v>
       </c>
       <c r="L5" s="24">
-        <f t="shared" ref="L5:L10" si="5">J5*K5*15/60</f>
+        <f t="shared" ref="L5:L10" si="9">J5*K5*15/60</f>
         <v>136.20000000000002</v>
       </c>
       <c r="M5" s="21"/>
-      <c r="N5" s="23"/>
+      <c r="N5" s="23">
+        <f t="shared" si="1"/>
+        <v>7.8819444444444432E-3</v>
+      </c>
       <c r="O5" s="23"/>
       <c r="P5" s="25"/>
       <c r="Q5" s="21"/>
       <c r="R5" s="24">
-        <f t="shared" ref="R5:R10" si="6">P5*Q5*15/60</f>
+        <f t="shared" ref="R5:R10" si="10">P5*Q5*15/60</f>
         <v>0</v>
       </c>
       <c r="S5" s="21"/>
-      <c r="T5" s="23"/>
+      <c r="T5" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="U5" s="23"/>
       <c r="V5" s="25"/>
       <c r="W5" s="21"/>
       <c r="X5" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y5" s="21"/>
-      <c r="Z5" s="23"/>
+      <c r="Z5" s="23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="AA5" s="23"/>
       <c r="AB5" s="25"/>
       <c r="AC5" s="21"/>
       <c r="AD5" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AE5" s="21" t="s">
         <v>29</v>
       </c>
       <c r="AF5" s="21">
-        <f t="shared" ref="AF5:AF10" si="7">IF(K5=0.8,L5*0.2,0)+IF(Q5=0.8,R5*0.2,0)+IF(W5=0.8,X5*0.2,0)+IF(AC5=0.8,AD5*0.2,0)</f>
+        <f t="shared" ref="AF5:AF10" si="11">IF(K5=0.8,L5*0.2,0)+IF(Q5=0.8,R5*0.2,0)+IF(W5=0.8,X5*0.2,0)+IF(AC5=0.8,AD5*0.2,0)</f>
         <v>27.240000000000006</v>
       </c>
       <c r="AG5" s="24">
-        <f t="shared" ref="AG5:AG10" si="8">(MINUTE(D5)*60+SECOND(D5))*10/60</f>
-        <v>113.5</v>
+        <f t="shared" si="6"/>
+        <v>140.74</v>
       </c>
       <c r="AH5" s="21" t="s">
         <v>32</v>
@@ -1377,7 +1402,7 @@
       </c>
       <c r="AL5" s="24">
         <f t="shared" si="0"/>
-        <v>338.75000000000006</v>
+        <v>365.99000000000007</v>
       </c>
       <c r="AM5" s="27"/>
       <c r="AN5" s="27"/>
@@ -1399,7 +1424,7 @@
         <v>30</v>
       </c>
       <c r="F6" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>41.55</v>
       </c>
       <c r="G6" s="21" t="s">
@@ -1412,86 +1437,89 @@
         <v>2.4189814814814816E-3</v>
       </c>
       <c r="J6" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>209</v>
       </c>
       <c r="K6" s="21">
         <v>0.8</v>
       </c>
       <c r="L6" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>41.800000000000004</v>
       </c>
       <c r="M6" s="21" t="s">
         <v>36</v>
       </c>
       <c r="N6" s="23">
-        <v>2.4305555555555556E-3</v>
+        <f t="shared" si="1"/>
+        <v>2.4189814814814816E-3</v>
       </c>
       <c r="O6" s="23">
         <v>4.8495370370370368E-3</v>
       </c>
       <c r="P6" s="25">
-        <f t="shared" ref="P6:P10" si="9">(MINUTE(O6)*60+SECOND(O6))-(MINUTE(N6)*60+SECOND(N6))</f>
-        <v>209</v>
+        <f t="shared" ref="P6:P10" si="12">(MINUTE(O6)*60+SECOND(O6))-(MINUTE(N6)*60+SECOND(N6))</f>
+        <v>210</v>
       </c>
       <c r="Q6" s="21">
         <v>1</v>
       </c>
       <c r="R6" s="24">
-        <f t="shared" si="6"/>
-        <v>52.25</v>
+        <f t="shared" si="10"/>
+        <v>52.5</v>
       </c>
       <c r="S6" s="21" t="s">
         <v>29</v>
       </c>
       <c r="T6" s="23">
-        <v>4.8611111111111112E-3</v>
+        <f t="shared" si="2"/>
+        <v>4.8495370370370368E-3</v>
       </c>
       <c r="U6" s="23">
         <v>7.2800925925925915E-3</v>
       </c>
       <c r="V6" s="25">
-        <f t="shared" ref="V6:V10" si="10">(MINUTE(U6)*60+SECOND(U6))-(MINUTE(T6)*60+SECOND(T6))</f>
-        <v>209</v>
+        <f t="shared" ref="V6:V10" si="13">(MINUTE(U6)*60+SECOND(U6))-(MINUTE(T6)*60+SECOND(T6))</f>
+        <v>210</v>
       </c>
       <c r="W6" s="21">
         <v>1</v>
       </c>
       <c r="X6" s="24">
-        <f t="shared" si="1"/>
-        <v>52.25</v>
+        <f t="shared" si="3"/>
+        <v>52.5</v>
       </c>
       <c r="Y6" s="21" t="s">
         <v>37</v>
       </c>
       <c r="Z6" s="23">
-        <v>7.2916666666666659E-3</v>
+        <f t="shared" si="4"/>
+        <v>7.2800925925925915E-3</v>
       </c>
       <c r="AA6" s="23">
         <v>9.4444444444444445E-3</v>
       </c>
       <c r="AB6" s="25">
-        <f t="shared" ref="AB6:AB8" si="11">(MINUTE(AA6)*60+SECOND(AA6))-(MINUTE(Z6)*60+SECOND(Z6))</f>
-        <v>186</v>
+        <f t="shared" ref="AB6:AB8" si="14">(MINUTE(AA6)*60+SECOND(AA6))-(MINUTE(Z6)*60+SECOND(Z6))</f>
+        <v>187</v>
       </c>
       <c r="AC6" s="21">
         <v>1</v>
       </c>
       <c r="AD6" s="24">
-        <f t="shared" si="2"/>
-        <v>46.5</v>
+        <f t="shared" si="5"/>
+        <v>46.75</v>
       </c>
       <c r="AE6" s="21" t="s">
         <v>30</v>
       </c>
       <c r="AF6" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>8.3600000000000012</v>
       </c>
       <c r="AG6" s="24">
-        <f t="shared" si="8"/>
-        <v>138.5</v>
+        <f t="shared" si="6"/>
+        <v>146.86000000000001</v>
       </c>
       <c r="AH6" s="21" t="s">
         <v>32</v>
@@ -1509,7 +1537,7 @@
       </c>
       <c r="AL6" s="24">
         <f t="shared" si="0"/>
-        <v>427.85</v>
+        <v>436.96000000000004</v>
       </c>
       <c r="AM6" s="27"/>
       <c r="AN6" s="27"/>
@@ -1531,7 +1559,7 @@
         <v>29</v>
       </c>
       <c r="F7" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>14.05</v>
       </c>
       <c r="G7" s="21" t="s">
@@ -1544,52 +1572,61 @@
         <v>3.2523148148148151E-3</v>
       </c>
       <c r="J7" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>281</v>
       </c>
       <c r="K7" s="21">
         <v>1</v>
       </c>
       <c r="L7" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>70.25</v>
       </c>
       <c r="M7" s="21"/>
-      <c r="N7" s="23"/>
+      <c r="N7" s="23">
+        <f t="shared" si="1"/>
+        <v>3.2523148148148151E-3</v>
+      </c>
       <c r="O7" s="23"/>
       <c r="P7" s="25"/>
       <c r="Q7" s="21"/>
       <c r="R7" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="S7" s="21"/>
-      <c r="T7" s="23"/>
+      <c r="T7" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="U7" s="23"/>
       <c r="V7" s="25"/>
       <c r="W7" s="21"/>
       <c r="X7" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y7" s="21"/>
-      <c r="Z7" s="23"/>
+      <c r="Z7" s="23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="AA7" s="23"/>
       <c r="AB7" s="25"/>
       <c r="AC7" s="21"/>
       <c r="AD7" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AE7" s="21" t="s">
         <v>31</v>
       </c>
       <c r="AF7" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG7" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>46.833333333333336</v>
       </c>
       <c r="AH7" s="21" t="s">
@@ -1630,7 +1667,7 @@
         <v>30</v>
       </c>
       <c r="F8" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>39.950000000000003</v>
       </c>
       <c r="G8" s="21" t="s">
@@ -1643,86 +1680,89 @@
         <v>2.2569444444444447E-3</v>
       </c>
       <c r="J8" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>195</v>
       </c>
       <c r="K8" s="21">
         <v>1</v>
       </c>
       <c r="L8" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>48.75</v>
       </c>
       <c r="M8" s="21" t="s">
         <v>35</v>
       </c>
       <c r="N8" s="23">
-        <v>2.2685185185185182E-3</v>
+        <f t="shared" si="1"/>
+        <v>2.2569444444444447E-3</v>
       </c>
       <c r="O8" s="23">
         <v>4.5138888888888893E-3</v>
       </c>
       <c r="P8" s="25">
-        <f t="shared" si="9"/>
-        <v>194</v>
+        <f t="shared" si="12"/>
+        <v>195</v>
       </c>
       <c r="Q8" s="21">
         <v>0.8</v>
       </c>
       <c r="R8" s="24">
-        <f t="shared" si="6"/>
-        <v>38.800000000000004</v>
+        <f t="shared" si="10"/>
+        <v>39</v>
       </c>
       <c r="S8" s="21" t="s">
         <v>40</v>
       </c>
       <c r="T8" s="23">
-        <v>4.5254629629629629E-3</v>
+        <f t="shared" si="2"/>
+        <v>4.5138888888888893E-3</v>
       </c>
       <c r="U8" s="23">
         <v>6.7708333333333336E-3</v>
       </c>
       <c r="V8" s="25">
         <f>(MINUTE(U8)*60+SECOND(U8))-(MINUTE(T8)*60+SECOND(T8))</f>
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="W8" s="21">
         <v>1</v>
       </c>
       <c r="X8" s="24">
-        <f t="shared" si="1"/>
-        <v>48.5</v>
+        <f t="shared" si="3"/>
+        <v>48.75</v>
       </c>
       <c r="Y8" s="21" t="s">
         <v>43</v>
       </c>
       <c r="Z8" s="23">
-        <v>6.782407407407408E-3</v>
+        <f t="shared" si="4"/>
+        <v>6.7708333333333336E-3</v>
       </c>
       <c r="AA8" s="23">
         <v>9.0972222222222218E-3</v>
       </c>
       <c r="AB8" s="25">
-        <f t="shared" si="11"/>
-        <v>200</v>
+        <f t="shared" si="14"/>
+        <v>201</v>
       </c>
       <c r="AC8" s="21">
         <v>0.8</v>
       </c>
       <c r="AD8" s="24">
-        <f t="shared" si="2"/>
-        <v>40</v>
+        <f t="shared" si="5"/>
+        <v>40.200000000000003</v>
       </c>
       <c r="AE8" s="21" t="s">
         <v>29</v>
       </c>
       <c r="AF8" s="21">
-        <f t="shared" si="7"/>
-        <v>15.760000000000002</v>
+        <f t="shared" si="11"/>
+        <v>15.840000000000002</v>
       </c>
       <c r="AG8" s="24">
-        <f t="shared" si="8"/>
-        <v>133.16666666666666</v>
+        <f t="shared" si="6"/>
+        <v>149.00666666666666</v>
       </c>
       <c r="AH8" s="21" t="s">
         <v>32</v>
@@ -1740,7 +1780,7 @@
       </c>
       <c r="AL8" s="24">
         <f t="shared" si="0"/>
-        <v>404.16666666666663</v>
+        <v>420.65666666666664</v>
       </c>
       <c r="AM8" s="27"/>
       <c r="AN8" s="27"/>
@@ -1762,7 +1802,7 @@
         <v>38</v>
       </c>
       <c r="F9" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>34.65</v>
       </c>
       <c r="G9" s="21" t="s">
@@ -1775,74 +1815,79 @@
         <v>2.5462962962962961E-3</v>
       </c>
       <c r="J9" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>220</v>
       </c>
       <c r="K9" s="21">
         <v>1</v>
       </c>
       <c r="L9" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>55</v>
       </c>
       <c r="M9" s="21" t="s">
         <v>41</v>
       </c>
       <c r="N9" s="23">
+        <f t="shared" si="1"/>
         <v>2.5462962962962961E-3</v>
       </c>
       <c r="O9" s="23">
         <v>5.0925925925925921E-3</v>
       </c>
       <c r="P9" s="25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>220</v>
       </c>
       <c r="Q9" s="21">
         <v>1</v>
       </c>
       <c r="R9" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>55</v>
       </c>
       <c r="S9" s="21" t="s">
         <v>35</v>
       </c>
       <c r="T9" s="23">
+        <f t="shared" si="2"/>
         <v>5.0925925925925921E-3</v>
       </c>
       <c r="U9" s="23">
         <v>7.858796296296296E-3</v>
       </c>
       <c r="V9" s="25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>239</v>
       </c>
       <c r="W9" s="21">
         <v>1</v>
       </c>
       <c r="X9" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>59.75</v>
       </c>
       <c r="Y9" s="21"/>
-      <c r="Z9" s="23"/>
+      <c r="Z9" s="23">
+        <f t="shared" si="4"/>
+        <v>7.858796296296296E-3</v>
+      </c>
       <c r="AA9" s="23"/>
       <c r="AB9" s="25"/>
       <c r="AC9" s="21"/>
       <c r="AD9" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AE9" s="21" t="s">
         <v>31</v>
       </c>
       <c r="AF9" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG9" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>115.5</v>
       </c>
       <c r="AH9" s="21" t="s">
@@ -1883,7 +1928,7 @@
         <v>29</v>
       </c>
       <c r="F10" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>37.6</v>
       </c>
       <c r="G10" s="21" t="s">
@@ -1896,75 +1941,80 @@
         <v>2.7777777777777801E-3</v>
       </c>
       <c r="J10" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>240</v>
       </c>
       <c r="K10" s="21">
         <v>1</v>
       </c>
       <c r="L10" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="M10" s="21" t="s">
         <v>35</v>
       </c>
       <c r="N10" s="23">
-        <v>2.7777777777777779E-3</v>
+        <f t="shared" si="1"/>
+        <v>2.7777777777777801E-3</v>
       </c>
       <c r="O10" s="23">
         <v>5.5555555555555558E-3</v>
       </c>
       <c r="P10" s="25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>240</v>
       </c>
       <c r="Q10" s="21">
         <v>0.8</v>
       </c>
       <c r="R10" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>48</v>
       </c>
       <c r="S10" s="21" t="s">
         <v>31</v>
       </c>
       <c r="T10" s="23">
+        <f t="shared" si="2"/>
         <v>5.5555555555555558E-3</v>
       </c>
       <c r="U10" s="23">
         <v>8.5416666666666679E-3</v>
       </c>
       <c r="V10" s="25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>258</v>
       </c>
       <c r="W10" s="21">
         <v>1</v>
       </c>
       <c r="X10" s="24">
-        <f t="shared" ref="X6:X10" si="12">V10*W10*15/60</f>
+        <f t="shared" ref="X10" si="15">V10*W10*15/60</f>
         <v>64.5</v>
       </c>
       <c r="Y10" s="21"/>
-      <c r="Z10" s="23"/>
+      <c r="Z10" s="23">
+        <f t="shared" si="4"/>
+        <v>8.5416666666666679E-3</v>
+      </c>
       <c r="AA10" s="23"/>
       <c r="AB10" s="25"/>
       <c r="AC10" s="21"/>
       <c r="AD10" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AE10" s="21" t="s">
         <v>29</v>
       </c>
       <c r="AF10" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>9.6000000000000014</v>
       </c>
       <c r="AG10" s="24">
-        <f t="shared" si="8"/>
-        <v>125.33333333333333</v>
+        <f t="shared" si="6"/>
+        <v>134.93333333333334</v>
       </c>
       <c r="AH10" s="21" t="s">
         <v>32</v>
@@ -1982,7 +2032,7 @@
       </c>
       <c r="AL10" s="24">
         <f t="shared" si="0"/>
-        <v>390.43333333333334</v>
+        <v>400.03333333333336</v>
       </c>
       <c r="AM10" s="27"/>
       <c r="AN10" s="27"/>

</xml_diff>

<commit_message>
v0.1.9 (2019/7/31 12:00) Added: 每月固定支出 在`config.py`中设置
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99132B0-24C6-4FF9-A7C2-6372B868C42E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861C787F-F5C7-410E-9D01-DF1DC247CDFE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -859,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE13" sqref="AE13"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AJ14" sqref="AJ14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
v0.2.1 (2019/9/8 23:25) Added Template.xlsx 方便进行统计
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70287B68-B04E-46E9-958D-2B66F008FDAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083D723D-0145-456B-B9D6-187245D2329A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -925,9 +926,9 @@
   <dimension ref="A1:AO12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <pane xSplit="8640" ySplit="8100" topLeftCell="AC28" activePane="topRight"/>
+      <pane xSplit="8640" ySplit="8100" topLeftCell="E28" activePane="topRight"/>
       <selection activeCell="T7" sqref="T7"/>
-      <selection pane="topRight" activeCell="AI9" sqref="AI9"/>
+      <selection pane="topRight" activeCell="F13" sqref="F13"/>
       <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
       <selection pane="bottomRight" activeCell="AD31" sqref="AD31"/>
     </sheetView>
@@ -1221,7 +1222,10 @@
       <c r="T3" s="17"/>
       <c r="U3" s="30"/>
       <c r="V3" s="30"/>
-      <c r="W3" s="20"/>
+      <c r="W3" s="20">
+        <f>IF(ISBLANK(T3),0,(MINUTE(V3)*60+SECOND(V3))-(MINUTE(U3)*60+SECOND(U3)))</f>
+        <v>0</v>
+      </c>
       <c r="X3" s="17"/>
       <c r="Y3" s="19">
         <f>IF(E3,1.25,1)*W3*(10+X3)/60</f>
@@ -1338,48 +1342,54 @@
       <c r="T4" s="17"/>
       <c r="U4" s="30"/>
       <c r="V4" s="30"/>
-      <c r="W4" s="20"/>
+      <c r="W4" s="20">
+        <f t="shared" ref="W4:W10" si="6">IF(ISBLANK(T4),0,(MINUTE(V4)*60+SECOND(V4))-(MINUTE(U4)*60+SECOND(U4)))</f>
+        <v>0</v>
+      </c>
       <c r="X4" s="17"/>
       <c r="Y4" s="19">
-        <f t="shared" ref="Y4:Y10" si="6">IF(E4,1.25,1)*W4*(10+X4)/60</f>
+        <f t="shared" ref="Y4:Y10" si="7">IF(E4,1.25,1)*W4*(10+X4)/60</f>
         <v>0</v>
       </c>
       <c r="Z4" s="17"/>
       <c r="AA4" s="30"/>
       <c r="AB4" s="30"/>
-      <c r="AC4" s="20"/>
+      <c r="AC4" s="20">
+        <f t="shared" ref="AC4:AC10" si="8">IF(ISBLANK(Z4),0,(MINUTE(AB4)*60+SECOND(AB4))-(MINUTE(AA4)*60+SECOND(AA4)))</f>
+        <v>0</v>
+      </c>
       <c r="AD4" s="17"/>
       <c r="AE4" s="19">
-        <f t="shared" ref="AE4:AE10" si="7">IF(E4,1.25,1)*AC4*(10+AD4)/60</f>
+        <f t="shared" ref="AE4:AE10" si="9">IF(E4,1.25,1)*AC4*(10+AD4)/60</f>
         <v>0</v>
       </c>
       <c r="AF4" s="17" t="s">
         <v>71</v>
       </c>
       <c r="AG4" s="20">
-        <f t="shared" ref="AG4:AG10" si="8">((60*MINUTE(D4)+SECOND(D4))*15/60)*IF(E4,1.25,1)-(AE4+Y4+S4+M4)</f>
+        <f t="shared" ref="AG4:AG10" si="10">((60*MINUTE(D4)+SECOND(D4))*15/60)*IF(E4,1.25,1)-(AE4+Y4+S4+M4)</f>
         <v>0</v>
       </c>
       <c r="AH4" s="19">
-        <f t="shared" ref="AH4:AH9" si="9">IF(E4,1.25,1)*(MINUTE(D4)*60+SECOND(D4))*10/60+AG4</f>
+        <f t="shared" ref="AH4:AH9" si="11">IF(E4,1.25,1)*(MINUTE(D4)*60+SECOND(D4))*10/60+AG4</f>
         <v>124.16666666666667</v>
       </c>
       <c r="AI4" s="17" t="s">
         <v>22</v>
       </c>
       <c r="AJ4" s="21">
-        <f t="shared" ref="AJ4:AJ10" si="10">IF(E4,1.25,1)*40</f>
+        <f t="shared" ref="AJ4:AJ10" si="12">IF(E4,1.25,1)*40</f>
         <v>40</v>
       </c>
       <c r="AK4" s="17" t="s">
         <v>73</v>
       </c>
       <c r="AL4" s="21">
-        <f t="shared" ref="AL4:AL9" si="11">IF(E4,1.25,1)*15</f>
+        <f t="shared" ref="AL4:AL9" si="13">IF(E4,1.25,1)*15</f>
         <v>15</v>
       </c>
       <c r="AM4" s="19">
-        <f t="shared" ref="AM4:AM9" si="12">AJ4+AL4+AH4+AE4+Y4+S4+M4+G4</f>
+        <f t="shared" ref="AM4:AM9" si="14">AJ4+AL4+AH4+AE4+Y4+S4+M4+G4</f>
         <v>402.66666666666669</v>
       </c>
       <c r="AN4" s="22"/>
@@ -1453,71 +1463,71 @@
         <v>74</v>
       </c>
       <c r="U5" s="30">
-        <f t="shared" ref="U5:U6" si="13">P5</f>
+        <f t="shared" ref="U5:U6" si="15">P5</f>
         <v>5.208333333333333E-3</v>
       </c>
       <c r="V5" s="30">
         <v>7.8703703703703713E-3</v>
       </c>
       <c r="W5" s="20">
-        <f t="shared" ref="W5:W10" si="14">IF(ISBLANK(T5),0,(MINUTE(V5)*60+SECOND(V5))-(MINUTE(U5)*60+SECOND(U5)))</f>
+        <f t="shared" si="6"/>
         <v>230</v>
       </c>
       <c r="X5" s="17">
         <v>4</v>
       </c>
       <c r="Y5" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>53.666666666666664</v>
       </c>
       <c r="Z5" s="17" t="s">
         <v>56</v>
       </c>
       <c r="AA5" s="30">
-        <f t="shared" ref="AA5" si="15">V5</f>
+        <f t="shared" ref="AA5" si="16">V5</f>
         <v>7.8703703703703713E-3</v>
       </c>
       <c r="AB5" s="30">
         <v>1.0613425925925927E-2</v>
       </c>
       <c r="AC5" s="20">
-        <f t="shared" ref="AC5:AC7" si="16">IF(ISBLANK(Z5),0,(MINUTE(AB5)*60+SECOND(AB5))-(MINUTE(AA5)*60+SECOND(AA5)))</f>
+        <f t="shared" si="8"/>
         <v>237</v>
       </c>
       <c r="AD5" s="17">
         <v>5</v>
       </c>
       <c r="AE5" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>59.25</v>
       </c>
       <c r="AF5" s="17" t="s">
         <v>21</v>
       </c>
       <c r="AG5" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>9.8333333333333428</v>
       </c>
       <c r="AH5" s="19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>166.66666666666669</v>
       </c>
       <c r="AI5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="AJ5" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>40</v>
       </c>
       <c r="AK5" s="17" t="s">
         <v>41</v>
       </c>
       <c r="AL5" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
       <c r="AM5" s="19">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>494.13333333333338</v>
       </c>
       <c r="AN5" s="22"/>
@@ -1591,64 +1601,64 @@
         <v>77</v>
       </c>
       <c r="U6" s="30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="V6" s="30">
         <v>1.0949074074074075E-2</v>
       </c>
       <c r="W6" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>346</v>
       </c>
       <c r="X6" s="17">
         <v>5</v>
       </c>
       <c r="Y6" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>108.125</v>
       </c>
       <c r="Z6" s="17"/>
       <c r="AA6" s="30"/>
       <c r="AB6" s="30"/>
       <c r="AC6" s="20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD6" s="17">
         <v>5</v>
       </c>
       <c r="AE6" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF6" s="17" t="s">
         <v>78</v>
       </c>
       <c r="AG6" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.25</v>
       </c>
       <c r="AH6" s="19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>203.33333333333334</v>
       </c>
       <c r="AI6" s="17" t="s">
         <v>22</v>
       </c>
       <c r="AJ6" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="AK6" s="17" t="s">
         <v>23</v>
       </c>
       <c r="AL6" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>18.75</v>
       </c>
       <c r="AM6" s="19">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>620.58333333333337</v>
       </c>
       <c r="AN6" s="22"/>
@@ -1727,14 +1737,14 @@
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="W7" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>240</v>
       </c>
       <c r="X7" s="17">
         <v>5</v>
       </c>
       <c r="Y7" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="Z7" s="17" t="s">
@@ -1747,7 +1757,7 @@
         <v>1.1087962962962964E-2</v>
       </c>
       <c r="AC7" s="20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="8"/>
         <v>238</v>
       </c>
       <c r="AD7" s="17">
@@ -1761,29 +1771,29 @@
         <v>55</v>
       </c>
       <c r="AG7" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AH7" s="19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>159.66666666666666</v>
       </c>
       <c r="AI7" s="17" t="s">
         <v>22</v>
       </c>
       <c r="AJ7" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>40</v>
       </c>
       <c r="AK7" s="17" t="s">
         <v>82</v>
       </c>
       <c r="AL7" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
       <c r="AM7" s="19">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>502.06666666666661</v>
       </c>
       <c r="AN7" s="22"/>
@@ -1856,48 +1866,54 @@
       <c r="T8" s="17"/>
       <c r="U8" s="30"/>
       <c r="V8" s="30"/>
-      <c r="W8" s="20"/>
+      <c r="W8" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="X8" s="17"/>
       <c r="Y8" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Z8" s="17"/>
       <c r="AA8" s="30"/>
       <c r="AB8" s="30"/>
-      <c r="AC8" s="20"/>
+      <c r="AC8" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="AD8" s="17"/>
       <c r="AE8" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF8" s="17" t="s">
         <v>21</v>
       </c>
       <c r="AG8" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AH8" s="19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>76.666666666666671</v>
       </c>
       <c r="AI8" s="17" t="s">
         <v>22</v>
       </c>
       <c r="AJ8" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>40</v>
       </c>
       <c r="AK8" s="17" t="s">
         <v>41</v>
       </c>
       <c r="AL8" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
       <c r="AM8" s="19">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>269.66666666666669</v>
       </c>
       <c r="AN8" s="22"/>
@@ -1970,48 +1986,54 @@
       <c r="T9" s="17"/>
       <c r="U9" s="30"/>
       <c r="V9" s="30"/>
-      <c r="W9" s="20"/>
+      <c r="W9" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="X9" s="17"/>
       <c r="Y9" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Z9" s="17"/>
       <c r="AA9" s="30"/>
       <c r="AB9" s="30"/>
-      <c r="AC9" s="20"/>
+      <c r="AC9" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="AD9" s="17"/>
       <c r="AE9" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF9" s="17" t="s">
         <v>78</v>
       </c>
       <c r="AG9" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AH9" s="19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>126.04166666666667</v>
       </c>
       <c r="AI9" s="17" t="s">
         <v>21</v>
       </c>
       <c r="AJ9" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="AK9" s="17" t="s">
         <v>41</v>
       </c>
       <c r="AL9" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>18.75</v>
       </c>
       <c r="AM9" s="19">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>421.66666666666669</v>
       </c>
       <c r="AN9" s="22"/>
@@ -2091,30 +2113,33 @@
         <v>7.0023148148148154E-3</v>
       </c>
       <c r="W10" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>205</v>
       </c>
       <c r="X10" s="17">
         <v>3</v>
       </c>
       <c r="Y10" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44.416666666666664</v>
       </c>
       <c r="Z10" s="17"/>
       <c r="AA10" s="30"/>
       <c r="AB10" s="30"/>
-      <c r="AC10" s="20"/>
+      <c r="AC10" s="20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="AD10" s="17"/>
       <c r="AE10" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF10" s="17" t="s">
         <v>77</v>
       </c>
       <c r="AG10" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>13.5</v>
       </c>
       <c r="AH10" s="19">
@@ -2125,7 +2150,7 @@
         <v>22</v>
       </c>
       <c r="AJ10" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>40</v>
       </c>
       <c r="AK10" s="17" t="s">

</xml_diff>